<commit_message>
Updating replication to test new bootstrapping
</commit_message>
<xml_diff>
--- a/replication/temp/table5_panel1.xlsx
+++ b/replication/temp/table5_panel1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>drink_def</t>
   </si>
@@ -37,46 +37,37 @@
     <t>police_report_only</t>
   </si>
   <si>
+    <t>(0.25)</t>
+  </si>
+  <si>
+    <t>(0.22)</t>
+  </si>
+  <si>
+    <t>any_evidence</t>
+  </si>
+  <si>
+    <t>(0.37)</t>
+  </si>
+  <si>
+    <t>(0.12)</t>
+  </si>
+  <si>
+    <t>police_report_primary</t>
+  </si>
+  <si>
+    <t>(0.01)</t>
+  </si>
+  <si>
     <t>(0.2)</t>
   </si>
   <si>
-    <t>(0.12)</t>
-  </si>
-  <si>
-    <t>any_evidence</t>
-  </si>
-  <si>
-    <t>(0.69)</t>
-  </si>
-  <si>
-    <t>(0.35)</t>
-  </si>
-  <si>
-    <t>police_report_primary</t>
-  </si>
-  <si>
-    <t>(0.21)</t>
-  </si>
-  <si>
-    <t>(0.03)</t>
-  </si>
-  <si>
     <t>bac_test_primary</t>
   </si>
   <si>
-    <t>(0.19)</t>
+    <t>multiple_imputation</t>
   </si>
   <si>
     <t>(0.05)</t>
-  </si>
-  <si>
-    <t>multiple_imputation</t>
-  </si>
-  <si>
-    <t>(0.11)</t>
-  </si>
-  <si>
-    <t>(0.04)</t>
   </si>
 </sst>
 </file>
@@ -474,7 +465,7 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -511,10 +502,10 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -551,10 +542,10 @@
         <v>14</v>
       </c>
       <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
         <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -574,7 +565,7 @@
         <v>3292</v>
       </c>
       <c r="F7">
-        <v>6733</v>
+        <v>6742</v>
       </c>
     </row>
   </sheetData>

</xml_diff>